<commit_message>
adding better version of templates with clacification
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>label</t>
   </si>
@@ -131,6 +131,45 @@
   </si>
   <si>
     <t>Often combined with joint locks for control transitions. Cultural significance in traditional Japanese martial arts.</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Submissions</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Joint Locks</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Wrist Locks</t>
+  </si>
+  <si>
+    <t>SubFamily</t>
+  </si>
+  <si>
+    <t>Flexion</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Gooseneck from Guard</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>Gooseneck form Half Guard</t>
   </si>
 </sst>
 </file>
@@ -558,6 +597,62 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>